<commit_message>
Adding draft R file of Lab 4 runtime stats
</commit_message>
<xml_diff>
--- a/Data_Structures/Data_Structures_Lab4_Fall2015/src/Lab4_RunningTimeStats.xlsx
+++ b/Data_Structures/Data_Structures_Lab4_Fall2015/src/Lab4_RunningTimeStats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="30200" yWindow="0" windowWidth="35840" windowHeight="20860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -952,19 +952,19 @@
   <dimension ref="A1:M193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:H9"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="34.5" customWidth="1"/>
+    <col min="1" max="1" width="84.6640625" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
     <col min="6" max="6" width="16.83203125" customWidth="1"/>
     <col min="7" max="7" width="18.6640625" customWidth="1"/>
-    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="8" max="8" width="36.83203125" customWidth="1"/>
     <col min="9" max="9" width="15.83203125" style="4" customWidth="1"/>
     <col min="10" max="10" width="17.33203125" style="5" customWidth="1"/>
     <col min="11" max="11" width="16.83203125" style="5" customWidth="1"/>
@@ -2509,7 +2509,6 @@
       <c r="D193" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1"/>
   <sortState ref="A2:M193">
     <sortCondition ref="B2:B193"/>
     <sortCondition ref="C2:C193"/>

</xml_diff>